<commit_message>
nb: running recording session day 3
</commit_message>
<xml_diff>
--- a/results/2023_05_27_cage_1_reward_training/proc/subject_and_date_rows_licking_specifity_output_directory/cage_1_date_20230526_20230528/subject_and_date_rows_licking_specifity_cage_1_date_20230526_20230528.xlsx
+++ b/results/2023_05_27_cage_1_reward_training/proc/subject_and_date_rows_licking_specifity_output_directory/cage_1_date_20230526_20230528/subject_and_date_rows_licking_specifity_cage_1_date_20230526_20230528.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -585,19 +585,19 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>1.3</v>
+        <v>1.2</v>
       </c>
       <c r="C7" t="n">
-        <v>20230526</v>
+        <v>20230528</v>
       </c>
       <c r="D7" t="n">
-        <v>0.002807692307692307</v>
+        <v>0.2377692307692308</v>
       </c>
       <c r="E7" t="n">
-        <v>0.000358974358974359</v>
+        <v>0.5196923076923078</v>
       </c>
       <c r="F7" t="n">
-        <v>20230526</v>
+        <v>20230528</v>
       </c>
       <c r="G7" t="n">
         <v>1</v>
@@ -611,16 +611,16 @@
         <v>1.3</v>
       </c>
       <c r="C8" t="n">
-        <v>20230527</v>
+        <v>20230526</v>
       </c>
       <c r="D8" t="n">
-        <v>0.120974358974359</v>
+        <v>0.002807692307692307</v>
       </c>
       <c r="E8" t="n">
-        <v>0.274025641025641</v>
+        <v>0.000358974358974359</v>
       </c>
       <c r="F8" t="n">
-        <v>20230527</v>
+        <v>20230526</v>
       </c>
       <c r="G8" t="n">
         <v>1</v>
@@ -631,19 +631,19 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>1.4</v>
+        <v>1.3</v>
       </c>
       <c r="C9" t="n">
-        <v>20230526</v>
+        <v>20230527</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0002692307692307692</v>
+        <v>0.120974358974359</v>
       </c>
       <c r="E9" t="n">
-        <v>0.000717948717948718</v>
+        <v>0.274025641025641</v>
       </c>
       <c r="F9" t="n">
-        <v>20230526</v>
+        <v>20230527</v>
       </c>
       <c r="G9" t="n">
         <v>1</v>
@@ -654,19 +654,19 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>1.4</v>
+        <v>1.3</v>
       </c>
       <c r="C10" t="n">
-        <v>20230527</v>
+        <v>20230528</v>
       </c>
       <c r="D10" t="n">
-        <v>0.1101025641025641</v>
+        <v>0.196051282051282</v>
       </c>
       <c r="E10" t="n">
-        <v>0.2383589743589744</v>
+        <v>0.3221025641025641</v>
       </c>
       <c r="F10" t="n">
-        <v>20230527</v>
+        <v>20230528</v>
       </c>
       <c r="G10" t="n">
         <v>1</v>
@@ -680,18 +680,64 @@
         <v>1.4</v>
       </c>
       <c r="C11" t="n">
+        <v>20230526</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.0002692307692307692</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.000717948717948718</v>
+      </c>
+      <c r="F11" t="n">
+        <v>20230526</v>
+      </c>
+      <c r="G11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="C12" t="n">
+        <v>20230527</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.1101025641025641</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.2383589743589744</v>
+      </c>
+      <c r="F12" t="n">
+        <v>20230527</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="C13" t="n">
         <v>20230528</v>
       </c>
-      <c r="D11" t="n">
+      <c r="D13" t="n">
         <v>0.1194871794871795</v>
       </c>
-      <c r="E11" t="n">
+      <c r="E13" t="n">
         <v>0.2931794871794872</v>
       </c>
-      <c r="F11" t="n">
+      <c r="F13" t="n">
         <v>20230528</v>
       </c>
-      <c r="G11" t="n">
+      <c r="G13" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>